<commit_message>
Tp Nro 5 terminado
</commit_message>
<xml_diff>
--- a/RepB_BIGRAMAS_TXTs.xlsx
+++ b/RepB_BIGRAMAS_TXTs.xlsx
@@ -462,17 +462,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.088</t>
+          <t>0.101</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Noticia N° 10.txt</t>
+          <t>Noticia N° 09.txt</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>título: taylor taylor swift: swift: estadounidense estadounidense puede puede ser ser barato barato verla verla buenos buenos aires aires comprar comprar ticket ticket ángeles ángeles resumen: resumen: alto alto costo costo entradas entradas presenciar presenciar show show artista artista país país origen origen generó generó polémica polémica fanáticos, fanáticos, portal portal financiero financiero eeuu eeuu recomendó recomendó venir venir recitales recitales argentina argentina contenido: contenido: jun, jun, medio medio quejas quejas alto alto costo costo venden venden unidos unidos entradas entradas tour tour exitosa exitosa cantante cantante taylor taylor swift, swift, sitio sitio finanzas finanzas norteamerincano norteamerincano hizo hizo llamativo llamativo cálculo: cálculo: portal portal estimó estimó cuánto cuánto cuesta cuesta viajar viajar angeles angeles buenos buenos aires aires comprar comprar tickets tickets presentación presentación cantante cantante argentina argentina vez vez comprar comprar tickets tickets ver ver actuación actuación ángleles. ángleles. conclusión conclusión sorprendente: sorprendente: aunque aunque computar computar estadía estadía comida, comida, costo costo pasaje pasaje avión avión compra compra entradas entradas recital recital buenos buenos aires aires resultó resultó combo combo económico económico ir ir verla verla país país origen. origen. según según morning morning brew brew “viajar “viajar avión avión angeles angeles buenos buenos aires aires comprar comprar tickets tickets ver ver cantante cantante pop pop taylor taylor swift swift barato barato estadounidense estadounidense ver ver artista artista propio propio país país “gracias “gracias inflación inflación argentina”. argentina”. acuerdo acuerdo precios precios publicados publicados cuenta cuenta twitter twitter sitio sitio especializado, especializado, @morningbrew, @morningbrew, comparación comparación precios precios siguiente: siguiente: precio precio entradas entradas ver ver taylor taylor swift swift angeles: angeles: dólares dólares pasajes pasajes aéreos aéreos ángeles ángeles buenos buenos aires: aires: dólares dólares valor valor entradas entradas concierto concierto buenos buenos aires: aires: dólares. dólares. “gracias “gracias inflación inflación argentina, argentina, realidad realidad barato barato alguien alguien ángeles ángeles volar volar argentina argentina concierto concierto tour tour ir ir estadio estadio sofi”, sofi”, indicó. indicó. cantante cantante pop pop estadounidense estadounidense taylor taylor swift swift presentará presentará argentina argentina dos dos conciertos conciertos estadio estadio river river plate plate noviembre noviembre próximos próximos marco marco gira gira internacional internacional “the “the tour”, tour”, informó informó través través comunicado comunicado prensa. prensa. según según anunció, anunció, entradas entradas ambos ambos shows shows venta venta clientes clientes banco banco patagonia patagonia hoy hoy horas horas agotar agotar stock, stock, suceda suceda primero, primero, venta venta general general comenzará comenzará mañana, mañana, martes martes junio junio precios, precios, podrán podrán pagar pagar cuotas cuotas tarjeta tarjeta entidad entidad bancaria bancaria promociana promociana recital, recital, parten parten $, $, ubicación ubicación denominada denominada centenario centenario alta alta visión visión restringida restringida detrás detrás escenario, escenario, puede puede disfrutar disfrutar música música aprecia aprecia totalidad totalidad show show $, $, entradas entradas caras. caras. dólares, dólares, tipo tipo cambio cambio libre, libre, precio precio menor menor usd usd entrada entrada costosa. costosa. gira gira internacional internacional comenzará comenzará agosto agosto tres tres fechas fechas ciudad ciudad méxico. méxico. luego, luego, tras tras dos dos conciertos conciertos estadio estadio river, river, presentaciones presentaciones continuarán continuarán brasil brasil show show noviembre noviembre río río janeiro janeiro dos dos mes mes san san pablo. pablo. todas todas fechas fechas américa américa latina, latina, taylor taylor swift swift contará contará cantante cantante norteamericana norteamericana sabrina sabrina carpenter carpenter invitada invitada especial. especial. seguir seguir leyendo leyendo urls urls imagenes:</t>
+          <t>título: aporte aporte dólar dólar soja, soja, banco banco central central compró compró solo solo usd usd millones millones mercado mercado resumen: resumen: entidad entidad monetaria monetaria encadenó encadenó ruedas ruedas operativas operativas compras compras netas, netas, margen margen achicó achicó primer primer día día agregado agregado tipo tipo cambio cambio especial especial exportaciones exportaciones sojeras sojeras contenido: contenido: jun, jun, sesión sesión usd usd millones millones segmento segmento contado contado spot, spot, liquidaciones liquidaciones programa programa incremento incremento exportador exportador economías economías regionales, regionales, dólar, dólar, aportaron aportaron usd usd millones, millones, volumen volumen aportado aportado ventas ventas soja soja derivados, derivados, gozaron gozaron estándar estándar cambiario cambiario semana semana pasada. pasada. bcra bcra concluyó concluyó intervención intervención cambiaria cambiaria día día saldo saldo neto neto comprador comprador solo solo millones millones dólares. dólares. operaciones operaciones dólar dólar agro agro registran registran tercera tercera etapa etapa ingresos ingresos usd usd millones millones abril abril parte. parte. asimismo, asimismo, empezó empezó balance balance bcra bcra intervención intervención cambiaria cambiaria negativo negativo usd usd millones, millones, mientras mientras junio junio sostiene sostiene im im saldo saldo comprador comprador millones millones dólares. dólares. bcra bcra aceleró aceleró resguardo resguardo escasas escasas reservas, reservas, medida medida afecta afecta provincias provincias municipios, municipios, momentos momentos ministerio ministerio economía economía planea planea nuevo nuevo canje canje voluntario voluntario bonos bonos pesos pesos objetivo objetivo despejar despejar vencimientos. vencimientos. ministro ministro economía, economía, sergio sergio massa, massa, viajará viajará washington washington cerca cerca junio junio procura procura cerrar cerrar readecuación readecuación acuerdo acuerdo fondo fondo monetario monetario internacional internacional fmi, fmi, permitiría permitiría argentina argentina obtener obtener adelanto adelanto desembolsos desembolsos nuevas nuevas metas metas cumplir, cumplir, luego luego impacto impacto sequía sequía exportaciones exportaciones sector sector agro, agro, “las “las negociaciones negociaciones argentina argentina funcionarios funcionarios técnicos técnicos fondo fondo avanzan avanzan hace hace casi casi dos dos meses meses través través reuniones reuniones virtuales, virtuales, definiendo definiendo modificar modificar viejo viejo acuerdo, acuerdo, virtualmente virtualmente suspendido suspendido luego luego cumplieran cumplieran metas metas reservas reservas fiscales fiscales primer primer trimestre trimestre ″, ″, comentaron comentaron expertos expertos research research traders. traders. objetivo objetivo economía economía fondo fondo adelante, adelante, menos, menos, parte parte desembolsos desembolsos comprometidos comprometidos fin fin año año usd usd millones, millones, ayudaría ayudaría reforzar reforzar reservas reservas año año exportaciones exportaciones sector sector agro agro caerían caerían cerca cerca usd usd millones, millones, acuerdo acuerdo proyecciones proyecciones bolsa bolsa comercio comercio rosario rosario bcr. bcr. tales tales desembolsos desembolsos dudas dudas cuánto cuánto podría podría utilizar utilizar intervenir intervenir mercado mercado cambiario. cambiario. fondo fondo aceptaría aceptaría bcra bcra intervenga intervenga eventuales eventuales situaciones situaciones stress. stress. todavía todavía resuelto resuelto monto monto fmi fmi consentiría consentiría intervenciones. intervenciones. reservas reservas internacionales internacionales brutas brutas banco banco central central crecieron crecieron semana semana pasada pasada usd usd millones millones finalizaron finalizaron millones millones dólares. dólares. informe informe anker anker latinoamérica latinoamérica subrayó subrayó cuanto cuanto reservas reservas líquidas líquidas bcra, bcra, “su “su disponibilidad disponibilidad hoy hoy dada dada gran gran medida medida encajes encajes cuentas cuentas bancarias bancarias monedas monedas depositados depositados bcra bcra -usd -usd millones-. millones-. estabilidad estabilidad depósitos depósitos moneda moneda extranjera extranjera crucial crucial sostener sostener capacidad capacidad intervención intervención bcra”. bcra”. luego luego diversas diversas gestiones gestiones ministro ministro massa massa incentivar incentivar pago pago importaciones importaciones divisa divisa china, china, expandió expandió uso uso yuanes yuanes comercio comercio exterior. exterior. enero enero mayo mayo operaciones operaciones equivalente equivalente usd usd millones. millones. además, además, dos dos empresas empresas fabricantes fabricantes electrónica electrónica confirmaron confirmaron pagarán pagarán compromisos compromisos deuda deuda total total usd usd millones millones moneda, moneda, alivio alivio arcas arcas bcra bcra superará superará usd usd millones millones primer primer trimestre trimestre seguir seguir leyendo: leyendo: urls urls imagenes:</t>
         </is>
       </c>
     </row>
@@ -482,7 +482,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.070</t>
+          <t>0.068</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -502,17 +502,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.068</t>
+          <t>0.053</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Noticia N° 05.txt</t>
+          <t>Noticia N° 06.txt</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>título: billetera billetera google google puede puede descargarse descargarse ser ser utilizada utilizada argentina argentina resumen: resumen: redes redes sociales sociales usuarios usuarios comentaron comentaron herramienta herramienta celulares celulares pudieron pudieron cargarle cargarle datos datos tarjetas tarjetas crédito crédito bancos bancos argentinos argentinos contenido: contenido: jun, jun, fernando fernando meaños meaños google google wallet, wallet, billetera billetera electrónica electrónica utilizada utilizada mundo mundo administrada administrada gigante gigante internet, internet, puede puede descargarse descargarse argentina argentina hacer hacer pagos pagos “contactless” “contactless” comercios comercios tarjetas tarjetas crédito crédito débito débito emitidas emitidas país. país. usuarios, usuarios, especial especial habituados habituados usar usar herramienta herramienta países, países, comenzaron comenzaron comentar comentar novedad novedad redes redes sociales sociales compartir compartir experiencias experiencias acerca acerca utilización. utilización. mecanismo mecanismo registrarse, registrarse, acuerdo acuerdo pudo pudo comprobar comprobar infobae, infobae, rápido rápido simple. simple. vez vez descargada descargada app app teléfono teléfono celular, celular, lleva lleva pocos pocos segundos, segundos, hace hace falta falta anotar anotar datos datos personales, personales, incluyendo incluyendo teléfono teléfono correo correo electrónico electrónico gmail. gmail. vez vez cumplido cumplido paso, paso, posible posible cargar cargar tarjetas tarjetas crédito crédito bancos bancos argentinos. argentinos. fin, fin, pide pide nuevo nuevo paso paso seguridad, seguridad, tal tal recibir recibir código código numérico numérico través través sms sms acreditar acreditar través través llamado llamado banco banco emisor. emisor. billetera billetera permite permite designarla designarla “medio “medio pago pago predeterminado” predeterminado” caso caso mismo mismo teléfono teléfono celular celular cargadas cargadas herramientas herramientas uso uso similar. similar. si si bien bien empresa empresa aún aún informó informó disponibilidad disponibilidad país país usuarios usuarios esperaban esperaban posibilidad posibilidad noticia noticia empezó empezó expandirse expandirse redes. redes. utilizaban utilizaban tarjetas tarjetas emitidas emitidas extranjero, extranjero, podrán podrán ahora ahora agregar agregar bancos bancos argentinos. argentinos. momento momento lanzamiento lanzamiento lugares lugares mundo, mundo, google google explicado explicado aplicación aplicación wallet wallet permite permite opciones opciones almacenar almacenar tarjetas tarjetas crédito crédito débito débito destinada destinada cargar cargar clase clase productos productos tarjetas tarjetas fidelidad fidelidad supermercados supermercados cadenas cadenas comerciales comerciales acumular acumular puntos puntos premios, premios, gift gift cards cards hacer hacer regalos, regalos, certificados certificados vacunación vacunación covid, covid, tarjetas tarjetas embarque embarque vuelo vuelo tarjetas tarjetas viajar viajar transporte transporte público. público. último, último, usuario usuario @mockelh @mockelh adelantó adelantó pedir: pedir: “salió “salió google google wallet wallet arg. arg. @tarjetasubeok @tarjetasubeok dale dale habilitá habilitá podamos podamos cargar cargar tarjeta tarjeta pagar pagar reloj”. reloj”. usuario usuario blog blog especializado especializado viajes, viajes, @sirchandlerblog, @sirchandlerblog, señaló: señaló: “esto “esto útil útil vida vida diaria, diaria, fundamental fundamental viajes. viajes. ciudades ciudades sistemas sistemas abiertos abiertos sube, sube, permiten permiten pago pago directo directo celulares celulares transporte transporte público. público. así así río río janeiro, janeiro, londres londres new new york”. york”. esperar esperar saber saber cuáles cuáles opciones opciones posibles posibles argentina. argentina. cierto cierto característica característica principal principal billetera billetera google google wallet wallet google google pay pay funciona funciona sistema sistema contactless contactless contacto, contacto, decir, decir, acercando acercando propio propio celular celular terminal terminal pos pos conocida conocida posnet, posnet, marcas marcas registre registre pago. pago. forma, forma, casos casos puede puede acortar acortar mínimo mínimo momento momento pago pago comparación comparación alternativas. alternativas. casi casi desuso desuso opción opción pagar pagar tarjeta, tarjeta, esperar esperar ticket ticket firmarlo, firmarlo, pago pago través través vía vía busca busca tener tener necesidad necesidad llevar llevar todas todas tarjetas tarjetas bolsillo bolsillo sino sino cargarlas cargarlas “digitalmente” “digitalmente” celular. celular. diferencia diferencia pagos pagos código código qr, qr, difundidos difundidos argentina, argentina, requieren requieren abrir abrir aplicación aplicación enfocar enfocar cámara cámara celular celular concretar concretar pago. pago. clave clave poder poder disponer disponer medio medio pago, pago, utilizado utilizado países países mundo, mundo, teléfono teléfono celular celular cuente cuente tecnología tecnología nfc, nfc, viene viene expandiéndose expandiéndose últimos últimos años años argentina. argentina. tecnología tecnología presente presente celulares celulares android android mercado mercado viabiliza viabiliza “pago “pago aproximación”, aproximación”, simplemente simplemente acercando acercando teléfono teléfono terminal terminal pos pos necesidad necesidad utilizar utilizar tarjeta tarjeta plástico. plástico. seguir seguir leyendo: leyendo: urls urls imagenes:</t>
+          <t>título: inflación inflación mayo mayo argentina argentina superó superó venezuela, venezuela, según según estimaciones estimaciones privadas privadas resumen: resumen: abril abril registrado registrado resultado; resultado; variado variado precios precios último último año año ambos ambos países países espera espera diciembre diciembre contenido: contenido: jun, jun, martín martín kanenguiser kanenguiser inflación inflación argentina argentina mayo mayo superó superó venezuela, venezuela, vez vez más, más, según según estimaciones estimaciones privadas privadas ambos ambos países. países. dato dato observatorio observatorio venezolano venezolano finanzas finanzas ovf, ovf, siguen siguen analistas analistas debido debido falta falta rigor rigor estadísticas estadísticas oficiales, oficiales, marcó marcó suba suba precios precios mes mes pasado, pasado, desaceleración desaceleración últimos últimos meses. meses. argentina, argentina, según según mayoría mayoría estimaciones, estimaciones, dato dato mes mes pasado pasado rondó rondó %, %, mientras mientras gobierno gobierno reza reza ubique ubique levemente levemente debajo debajo cifra. cifra. abril, abril, argentina argentina superado superado venezuela: venezuela: registró registró %, %, frente frente informado informado ovf ovf informado informado banco banco central central venezuela, venezuela, daba daba conocer conocer información información octubre octubre año año pasado. pasado. últimos últimos meses meses mayo-mayo, mayo-mayo, según según ovf, ovf, inflación inflación país país gobernado gobernado nicolás nicolás maduro maduro llegó llegó %, %, baja baja respecto respecto registrado registrado abril. abril. además, además, enero enero suba suba precios precios acumulada acumulada %. %. tendencias tendencias inflación inflación últimos últimos meses meses divergentes: divergentes: marzo marzo ovf ovf registró registró venezuela venezuela %, %, abril abril mayo mayo %; %; tanto, tanto, indec indec registró registró argentina argentina marzo, marzo, abril abril estima estima mes mes quedará quedará torno torno interanual; interanual; conocerá conocerá dato dato organismo organismo lidera lidera marco marco lavagna. lavagna. según según ovf, ovf, “en “en medio medio economía economía evidentes evidentes signos signos contracción, contracción, tasa tasa inflación inflación da da tregua. tregua. así, así, mayo mayo tasa tasa inflación inflación mensual mensual alcanzó alcanzó %, %, acumulada acumulada anualizada anualizada %. %. respecto respecto abril, abril, tasa tasa mensual mensual inflación inflación triplicó triplicó aunque aunque tasa tasa doce doce meses meses desaceleró”. desaceleró”. “este “este comportamiento comportamiento inflación inflación ocurriendo ocurriendo entorno entorno signos signos significativa significativa caída caída nivel nivel actividad actividad indiscutibles, indiscutibles, ostensibles ostensibles menores menores ventas ventas comercio comercio producción producción industrial industrial contrajo contrajo primer primer trimestre trimestre ″, ″, indicó. indicó. además, además, “la “la debilidad debilidad demanda demanda agregada agregada notoria notoria debido debido salarios salarios pensiones pensiones sector sector público público pronunciadamente pronunciadamente rezagados rezagados respecto respecto inflación inflación ejecución ejecución gasto gasto parte parte gobierno gobierno baja”. baja”. “al “al comparar comparar cifra cifra inflación inflación mayo mayo respecto respecto aumento aumento tipo tipo cambio cambio mismo mismo mes, mes, clara clara estrecha estrecha relación relación ambas ambas variables, variables, obstante, obstante, mencionó, mencionó, debilidad debilidad demanda, demanda, explicada explicada política política compresión compresión salarial salarial venido venido aplicando aplicando gobierno”, gobierno”, subrayó subrayó ovf. ovf. cuanto cuanto principales principales componentes componentes conforman conforman índice índice nacional nacional precios precios consumidor, consumidor, destacaron destacaron “los “los aumentos aumentos experimentados experimentados rubros rubros esparcimiento esparcimiento %, %, vestido vestido calzado calzado %, %, equipamiento equipamiento hogar hogar alquiler alquiler vivienda vivienda %. %. alimentos alimentos alzas alzas modestas, modestas, mayo mayo incrementaron incrementaron %”. %”. “todo “todo ello ello pone pone manifiesto, manifiesto, política política económica económica aplicada aplicada sido sido ineficaz ineficaz contener contener alza alza precios, precios, aún aún retracción retracción inducida inducida demanda demanda agregada”, agregada”, concluyó concluyó organismo organismo independiente independiente régimen régimen autoritario autoritario maduro. maduro. abril, abril, banco banco central central venezuela venezuela informado informado aumento aumento cuatro cuatro meses, meses, luego luego difundir difundir datos datos medio medio año. año. tanto, tanto, mayoría mayoría relevamientos relevamientos precios precios consumidor consumidor consultoras consultoras argentinas argentinas anticipan anticipan ipc ipc torno torno %. %. c&amp;t c&amp;t indicó indicó relevamiento relevamiento precios precios minoristas minoristas región región gba gba “presentó “presentó alza alza mensual mensual %, %, superando superando largamente largamente variación variación abril abril mayo mayo año año pasado. pasado. así, así, variación variación doce doce meses meses trepó trepó %, %, mayor mayor agosto agosto ″. ″. “el “el rubro rubro mayor mayor incremento incremento vivienda vivienda %, %, reflejando reflejando subas subas gas gas electricidad electricidad principalmente”, principalmente”, aclaró. aclaró. bienes bienes servicios servicios varios varios “ocuparon “ocuparon segundo segundo lugar, lugar, alza alza %, %, explicada explicada cigarrillos cigarrillos artículos artículos tocador”. tocador”. tanto, tanto, “el “el comportamiento comportamiento esparcimiento esparcimiento fuertemente fuertemente influido influido alza alza dólares dólares financieros financieros fines fines abril, abril, vio vio reflejado reflejado turismo turismo productos productos electrónicos”. electrónicos”. vez, vez, “alimentos “alimentos bebidas bebidas creció creció mes. mes. arrancó arrancó mes mes gran gran impulso impulso luego luego moderando. moderando. verduras, verduras, lácteos lácteos derivados derivados harina harina destacaron, destacaron, igual igual alimentos alimentos consumidos consumidos hogar hogar llevar”. llevar”. “en “en salud salud destacó destacó incremento incremento medicamentos, medicamentos, sumó sumó nuevo nuevo ajuste ajuste prepagas”, prepagas”, indicó indicó c&amp;t. c&amp;t. “en “en equipamiento equipamiento mantenimiento mantenimiento hogar, hogar, artefactos artefactos hogar hogar rol rol preponderante preponderante mano mano alza alza dólares dólares financieros financieros pesar pesar liquidaciones liquidaciones mes”, mes”, concluyó. concluyó. parte, parte, ecogo ecogo informó informó si si bien bien última última semana semana mes mes pasado pasado registró registró fuerte fuerte desaceleración desaceleración lugar lugar variación variación alimentos alimentos respecto respecto semana semana anterior, anterior, términos términos generales generales inflación inflación sido sido ciento. ciento. particular, particular, aumento aumento precios precios alimentos alimentos sido sido ciento. ciento. “si “si consideramos consideramos además además evolución evolución alimentos alimentos consumidos consumidos hogar hogar %, %, inflación inflación alimentos alimentos alcanzaría alcanzaría %”, %”, aclaró aclaró consultora consultora dirige dirige marina marina dal dal poggeto. poggeto. lado, lado, lcg lcg detalló detalló “el “el índice índice alimentos alimentos bebidas bebidas presentó presentó inflación inflación mensual mensual promedio promedio últimas últimas semanas semanas punta punta punta punta mismo mismo período”. período”. mes mes sumarán sumarán aumentos aumentos precios precios servicios servicios transporte, transporte, prepagas, prepagas, colegios colegios privados privados combustibles, combustibles, valores valores regulados. regulados. equipo equipo económico económico trata trata controlar controlar cuestión cuestión cambiaria cambiaria inflación inflación acelere acelere todavía todavía motivo motivo resiste resiste pedido pedido fmi fmi acelerar acelerar devaluación devaluación tipo tipo cambio cambio oficial. oficial. seguir seguir leyendo: leyendo: urls urls imagenes:</t>
         </is>
       </c>
     </row>

</xml_diff>